<commit_message>
Adding Test Classes: Login, MypersonalInfo, Addresses and Wishlist
</commit_message>
<xml_diff>
--- a/Test Plan/TestCase.xlsx
+++ b/Test Plan/TestCase.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7815" activeTab="2"/>
+    <workbookView windowWidth="20490" windowHeight="7815"/>
   </bookViews>
   <sheets>
     <sheet name="TS" sheetId="1" r:id="rId1"/>
     <sheet name="login" sheetId="2" r:id="rId2"/>
     <sheet name="My address" sheetId="4" r:id="rId3"/>
+    <sheet name="My personal info" sheetId="5" r:id="rId4"/>
+    <sheet name="My wishlist" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="182">
   <si>
     <t>Environment: Google Chrome  version</t>
   </si>
@@ -248,6 +250,9 @@
     <t>Authentication page is opened, and "Sign in" button is visible in the header</t>
   </si>
   <si>
+    <t>ID: 5</t>
+  </si>
+  <si>
     <t xml:space="preserve">TC name: Signing in with no credentials </t>
   </si>
   <si>
@@ -267,6 +272,9 @@
     <t>An email address required.</t>
   </si>
   <si>
+    <t>ID: 6</t>
+  </si>
+  <si>
     <t>TC name: Valdation of updating address in my address section</t>
   </si>
   <si>
@@ -288,13 +296,43 @@
     <t>In address field clear existing address and write a new address</t>
   </si>
   <si>
+    <t>Vršačka 4</t>
+  </si>
+  <si>
     <t>JNA 39</t>
   </si>
   <si>
-    <t>In City field clear existing City and write a new data</t>
-  </si>
-  <si>
-    <t>Čačak</t>
+    <t>In the address title box clear existing and write a new title for a new address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">My address </t>
+  </si>
+  <si>
+    <t xml:space="preserve">My changed address </t>
+  </si>
+  <si>
+    <t>Click on the green "Save" button in the end off personal information list</t>
+  </si>
+  <si>
+    <t>The address box is apered with valid credentials</t>
+  </si>
+  <si>
+    <t>ID: 7</t>
+  </si>
+  <si>
+    <t>TC name: Valdation of adding new address in my address section</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on the "Add a new address" green button </t>
+  </si>
+  <si>
+    <t>In address field write a new address</t>
+  </si>
+  <si>
+    <t>In City field write a new data</t>
+  </si>
+  <si>
+    <t>Novi Sad</t>
   </si>
   <si>
     <t>the field goes green after</t>
@@ -309,18 +347,18 @@
     <t>Click on the selected state</t>
   </si>
   <si>
+    <t>Ohio</t>
+  </si>
+  <si>
     <t>State is selected and drop down list is closed and box goes green</t>
   </si>
   <si>
-    <t>In zip/postal code box  clear existing and write new postal code</t>
+    <t>In zip/postal code box write postal code</t>
   </si>
   <si>
     <t>Click on the drop down list for selecting Country</t>
   </si>
   <si>
-    <t>Ohio</t>
-  </si>
-  <si>
     <t>The drop down list is opened</t>
   </si>
   <si>
@@ -333,42 +371,6 @@
     <t>Country is selected and drop down list is closed and box goes green</t>
   </si>
   <si>
-    <t>In the "Home phone" box  clear existing and write a new phone number</t>
-  </si>
-  <si>
-    <t>021762191</t>
-  </si>
-  <si>
-    <t>In the address title box clear existing and write a new title for a new address</t>
-  </si>
-  <si>
-    <t>My address new</t>
-  </si>
-  <si>
-    <t>Click on the green "Save" button in the end off personal information list</t>
-  </si>
-  <si>
-    <t>The address box is apered with valid credentials</t>
-  </si>
-  <si>
-    <t>TC name: Valdation of adding new address in my address section</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Click on the "Add a new address" grey button </t>
-  </si>
-  <si>
-    <t>In address field write a new address</t>
-  </si>
-  <si>
-    <t>In City field write a new data</t>
-  </si>
-  <si>
-    <t>Novi Sad</t>
-  </si>
-  <si>
-    <t>In zip/postal code box write postal code</t>
-  </si>
-  <si>
     <t>In the "Home phone" box write a phone number</t>
   </si>
   <si>
@@ -378,7 +380,193 @@
     <t>In the address title box write a title for a new address</t>
   </si>
   <si>
+    <t>MY ADDITIONAL ADDRESS</t>
+  </si>
+  <si>
     <t>Both "My Address" boxes are visible, with valid credentials</t>
+  </si>
+  <si>
+    <t>ID: 8</t>
+  </si>
+  <si>
+    <t>TC name: Valdation of deleting a new address in my address section</t>
+  </si>
+  <si>
+    <t>User is signed in and second address is added</t>
+  </si>
+  <si>
+    <t>Click "Delete" button under "Second address" section</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Message " Are you sure?" is displayed </t>
+  </si>
+  <si>
+    <t>Click "OK" button on the "Are you sure?" message</t>
+  </si>
+  <si>
+    <t>Secondary address is susccessfully deleted</t>
+  </si>
+  <si>
+    <t>ID: 9</t>
+  </si>
+  <si>
+    <t>TC name: Validation of editing first name in personal information section</t>
+  </si>
+  <si>
+    <t>Click on the fourth box link list saying "My personal information"</t>
+  </si>
+  <si>
+    <t>My personal information page is opened</t>
+  </si>
+  <si>
+    <t>Clear existing and enter another first name in the field "First name"</t>
+  </si>
+  <si>
+    <t>Jovančica</t>
+  </si>
+  <si>
+    <t>First name has been changed</t>
+  </si>
+  <si>
+    <t>Click on the lastname field</t>
+  </si>
+  <si>
+    <t>Broz</t>
+  </si>
+  <si>
+    <t>Last name stayed unchanged and field goes green</t>
+  </si>
+  <si>
+    <t>Clear existing and enter another email address in the field "Email address"</t>
+  </si>
+  <si>
+    <t>Email stayed unchanged and field goes green</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter current password </t>
+  </si>
+  <si>
+    <t>Password is correct</t>
+  </si>
+  <si>
+    <t>Click on "Save"</t>
+  </si>
+  <si>
+    <t>Your personal information has been successfully updated.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Message "Your personal informationhas been successfully updated" is displayed </t>
+  </si>
+  <si>
+    <t>ID: 10</t>
+  </si>
+  <si>
+    <t>TC name: Validation of editing lastfirst name in personal information section</t>
+  </si>
+  <si>
+    <t>Jovanka</t>
+  </si>
+  <si>
+    <t>First stayed unchanged and field goes green</t>
+  </si>
+  <si>
+    <t>Clear existing and enter another last name in the field "Last name"</t>
+  </si>
+  <si>
+    <t>Budisavljević</t>
+  </si>
+  <si>
+    <t>Last name has been changed</t>
+  </si>
+  <si>
+    <t>ID: 11</t>
+  </si>
+  <si>
+    <t>TC name: Validation of editing eMail in personal information section</t>
+  </si>
+  <si>
+    <t>budisavljevic@yahoo.com</t>
+  </si>
+  <si>
+    <t>Email has been changed</t>
+  </si>
+  <si>
+    <t>ID: 12</t>
+  </si>
+  <si>
+    <t>TC name: Validation of editing password in personal information section</t>
+  </si>
+  <si>
+    <t>First name stayed unchanged and field goes green</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter new password </t>
+  </si>
+  <si>
+    <t>#Rankovic</t>
+  </si>
+  <si>
+    <t>ID: 13</t>
+  </si>
+  <si>
+    <t>TC name: Validation of creating a wishlist</t>
+  </si>
+  <si>
+    <t>Click on the fourth section saying "My wishlist"</t>
+  </si>
+  <si>
+    <t>My wishlist page is opened</t>
+  </si>
+  <si>
+    <t>Enter name of the wishlist in the field "Name"</t>
+  </si>
+  <si>
+    <t>Šeširi</t>
+  </si>
+  <si>
+    <t>Name of the wishlist is visible</t>
+  </si>
+  <si>
+    <t>Click on the "Save" button</t>
+  </si>
+  <si>
+    <t>Section with a new wishlist is created</t>
+  </si>
+  <si>
+    <t>ID: 14</t>
+  </si>
+  <si>
+    <t>TC name: Validation of creating a multiple wishlists</t>
+  </si>
+  <si>
+    <t>Ogrtaci</t>
+  </si>
+  <si>
+    <t>Sunčane nočare</t>
+  </si>
+  <si>
+    <t>ID: 15</t>
+  </si>
+  <si>
+    <t>TC name: Validation of removing  wishlist</t>
+  </si>
+  <si>
+    <t>User is signed in, and one wishlist is made</t>
+  </si>
+  <si>
+    <t>Click on the "X" button on the right side</t>
+  </si>
+  <si>
+    <t>Message "Do you really want to delete this wishlist?" is displayed</t>
+  </si>
+  <si>
+    <t>Click on "OK" button</t>
+  </si>
+  <si>
+    <t>Successfully deleted</t>
+  </si>
+  <si>
+    <t>Message "Successfully deleted" is displayed</t>
   </si>
 </sst>
 </file>
@@ -388,10 +576,10 @@
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="32">
+  <fonts count="33">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -424,6 +612,22 @@
       <color theme="1"/>
       <name val="Arial"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -476,6 +680,35 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -484,7 +717,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -498,100 +754,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -613,8 +777,40 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -629,7 +825,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -641,7 +837,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -653,13 +915,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -671,13 +969,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -689,67 +987,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -761,55 +1005,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -820,6 +1016,54 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -843,21 +1087,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -887,43 +1116,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -941,134 +1137,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="25" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1084,30 +1280,38 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="7" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="7" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1430,8 +1634,8 @@
   <sheetPr/>
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1446,7 +1650,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3"/>
@@ -1460,19 +1664,19 @@
       <c r="J1" s="3"/>
     </row>
     <row r="2" ht="21" spans="1:10">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="21" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="4"/>
@@ -1505,7 +1709,7 @@
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="22" t="s">
         <v>11</v>
       </c>
       <c r="B8" t="s">
@@ -1538,7 +1742,7 @@
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="18"/>
+      <c r="A14" s="22"/>
       <c r="B14" t="s">
         <v>18</v>
       </c>
@@ -1549,19 +1753,19 @@
       </c>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16" s="18"/>
+      <c r="A16" s="22"/>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="18"/>
+      <c r="A18" s="22"/>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="18"/>
+      <c r="A20" s="22"/>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" s="18"/>
+      <c r="A22" s="22"/>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" s="18"/>
+      <c r="A24" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1577,8 +1781,8 @@
   <sheetPr/>
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37:G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1696,7 +1900,7 @@
       <c r="C8" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="12" t="s">
         <v>44</v>
       </c>
       <c r="G8" t="s">
@@ -1718,7 +1922,7 @@
       <c r="C10" t="s">
         <v>49</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="13" t="s">
         <v>50</v>
       </c>
       <c r="G10" t="s">
@@ -1792,8 +1996,6 @@
       <c r="D16" t="s">
         <v>34</v>
       </c>
-      <c r="E16"/>
-      <c r="F16"/>
       <c r="G16" t="s">
         <v>35</v>
       </c>
@@ -1805,8 +2007,6 @@
       <c r="D17" t="s">
         <v>37</v>
       </c>
-      <c r="E17"/>
-      <c r="F17"/>
       <c r="G17" t="s">
         <v>38</v>
       </c>
@@ -1815,9 +2015,6 @@
       <c r="C18" t="s">
         <v>39</v>
       </c>
-      <c r="D18"/>
-      <c r="E18"/>
-      <c r="F18"/>
       <c r="G18" t="s">
         <v>40</v>
       </c>
@@ -1826,9 +2023,6 @@
       <c r="C19" t="s">
         <v>41</v>
       </c>
-      <c r="D19"/>
-      <c r="E19"/>
-      <c r="F19"/>
       <c r="G19" t="s">
         <v>42</v>
       </c>
@@ -1837,11 +2031,9 @@
       <c r="C20" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E20"/>
-      <c r="F20"/>
       <c r="G20" t="s">
         <v>45</v>
       </c>
@@ -1853,7 +2045,6 @@
       <c r="E21" t="s">
         <v>54</v>
       </c>
-      <c r="F21"/>
       <c r="G21" t="s">
         <v>48</v>
       </c>
@@ -1862,9 +2053,7 @@
       <c r="C22" t="s">
         <v>49</v>
       </c>
-      <c r="D22"/>
-      <c r="E22"/>
-      <c r="F22" s="12" t="s">
+      <c r="F22" s="16" t="s">
         <v>55</v>
       </c>
       <c r="G22" t="s">
@@ -1872,7 +2061,7 @@
       </c>
     </row>
     <row r="23" spans="6:6">
-      <c r="F23" s="13" t="s">
+      <c r="F23" s="17" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1978,7 +2167,7 @@
       <c r="C32" t="s">
         <v>43</v>
       </c>
-      <c r="E32" s="8" t="s">
+      <c r="E32" s="12" t="s">
         <v>60</v>
       </c>
       <c r="G32" t="s">
@@ -2000,7 +2189,7 @@
       <c r="C34" t="s">
         <v>49</v>
       </c>
-      <c r="F34" s="12" t="s">
+      <c r="F34" s="16" t="s">
         <v>61</v>
       </c>
       <c r="G34" t="s">
@@ -2017,7 +2206,7 @@
       </c>
     </row>
     <row r="35" spans="6:6">
-      <c r="F35" s="14" t="s">
+      <c r="F35" s="18" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2090,8 +2279,6 @@
       <c r="D40" t="s">
         <v>69</v>
       </c>
-      <c r="E40"/>
-      <c r="F40"/>
       <c r="G40" t="s">
         <v>35</v>
       </c>
@@ -2108,8 +2295,6 @@
       <c r="D41" t="s">
         <v>71</v>
       </c>
-      <c r="E41"/>
-      <c r="F41"/>
       <c r="G41" t="s">
         <v>72</v>
       </c>
@@ -2130,13 +2315,13 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="1" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -2213,36 +2398,35 @@
     </row>
     <row r="52" spans="3:7">
       <c r="C52" t="s">
-        <v>77</v>
-      </c>
-      <c r="E52" s="8"/>
+        <v>78</v>
+      </c>
+      <c r="E52" s="12"/>
       <c r="G52" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="53" spans="3:7">
       <c r="C53" t="s">
+        <v>80</v>
+      </c>
+      <c r="G53" t="s">
         <v>79</v>
-      </c>
-      <c r="D53"/>
-      <c r="G53" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="54" ht="45" spans="3:7">
       <c r="C54" t="s">
         <v>49</v>
       </c>
-      <c r="F54" s="15" t="s">
-        <v>80</v>
+      <c r="F54" s="19" t="s">
+        <v>81</v>
       </c>
       <c r="G54" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="55" spans="6:6">
-      <c r="F55" s="14" t="s">
-        <v>81</v>
+      <c r="F55" s="18" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -2266,10 +2450,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A28" sqref="$A28:$XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -2287,13 +2471,13 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>83</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -2369,29 +2553,32 @@
     </row>
     <row r="6" customFormat="1" spans="3:7">
       <c r="C6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G6" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" customFormat="1" spans="3:7">
       <c r="C7" t="s">
-        <v>86</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>87</v>
+        <v>88</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="8" customFormat="1" spans="3:7">
       <c r="C8" t="s">
-        <v>88</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="E8" t="s">
+        <v>92</v>
       </c>
       <c r="G8" t="s">
         <v>45</v>
@@ -2399,181 +2586,195 @@
     </row>
     <row r="9" customFormat="1" spans="3:7">
       <c r="C9" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D9" t="s">
-        <v>91</v>
+        <v>94</v>
+      </c>
+      <c r="E9" t="s">
+        <v>95</v>
       </c>
       <c r="G9" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" customFormat="1" spans="3:7">
       <c r="C10" t="s">
-        <v>93</v>
-      </c>
-      <c r="F10" s="9"/>
+        <v>96</v>
+      </c>
       <c r="G10" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="11" spans="3:7">
-      <c r="C11" t="s">
-        <v>95</v>
-      </c>
-      <c r="D11"/>
-      <c r="G11" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="12" spans="3:7">
-      <c r="C12" t="s">
         <v>97</v>
       </c>
-      <c r="D12" s="10">
-        <v>11000</v>
-      </c>
-      <c r="G12" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="13" spans="3:7">
-      <c r="C13" t="s">
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D13" t="s">
+      <c r="B13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="G13" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="3:7">
-      <c r="C14" t="s">
-        <v>101</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="G14" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="15" spans="3:7">
-      <c r="C15" t="s">
-        <v>104</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="G15" t="s">
-        <v>45</v>
-      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" s="3"/>
     </row>
     <row r="16" spans="3:7">
       <c r="C16" t="s">
-        <v>106</v>
+        <v>68</v>
       </c>
       <c r="D16" t="s">
-        <v>107</v>
+        <v>69</v>
       </c>
       <c r="G16" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="3:7">
       <c r="C17" t="s">
-        <v>108</v>
+        <v>70</v>
+      </c>
+      <c r="D17" t="s">
+        <v>71</v>
       </c>
       <c r="G17" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="20" spans="3:8">
-      <c r="C20" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="4:8">
-      <c r="D21" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="H21" s="5"/>
-    </row>
-    <row r="22" spans="3:8">
-      <c r="C22" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H22" s="3"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7">
+      <c r="C18" t="s">
+        <v>85</v>
+      </c>
+      <c r="F18" t="s">
+        <v>86</v>
+      </c>
+      <c r="G18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7">
+      <c r="C19" t="s">
+        <v>100</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7">
+      <c r="C20" t="s">
+        <v>101</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="G20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7">
+      <c r="C21" t="s">
+        <v>102</v>
+      </c>
+      <c r="D21" t="s">
+        <v>103</v>
+      </c>
+      <c r="G21" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7">
+      <c r="C22" t="s">
+        <v>105</v>
+      </c>
+      <c r="F22" s="13"/>
+      <c r="G22" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="23" spans="3:7">
       <c r="C23" t="s">
-        <v>68</v>
+        <v>107</v>
       </c>
       <c r="D23" t="s">
-        <v>69</v>
+        <v>108</v>
       </c>
       <c r="G23" t="s">
-        <v>35</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="3:7">
       <c r="C24" t="s">
-        <v>70</v>
-      </c>
-      <c r="D24" t="s">
-        <v>71</v>
+        <v>110</v>
+      </c>
+      <c r="D24" s="14">
+        <v>21000</v>
       </c>
       <c r="G24" t="s">
-        <v>72</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="3:7">
       <c r="C25" t="s">
-        <v>83</v>
-      </c>
-      <c r="F25" t="s">
-        <v>84</v>
+        <v>111</v>
       </c>
       <c r="G25" t="s">
-        <v>85</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="3:7">
       <c r="C26" t="s">
-        <v>111</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>87</v>
+        <v>113</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="G26" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="3:7">
       <c r="C27" t="s">
-        <v>112</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>89</v>
+        <v>116</v>
+      </c>
+      <c r="D27" s="23" t="s">
+        <v>117</v>
       </c>
       <c r="G27" t="s">
         <v>45</v>
@@ -2581,103 +2782,1413 @@
     </row>
     <row r="28" spans="3:7">
       <c r="C28" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="D28" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="G28" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="3:7">
       <c r="C29" t="s">
-        <v>93</v>
-      </c>
-      <c r="F29" s="9"/>
+        <v>96</v>
+      </c>
       <c r="G29" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="30" spans="3:7">
-      <c r="C30" t="s">
-        <v>95</v>
-      </c>
-      <c r="D30" t="s">
-        <v>99</v>
-      </c>
-      <c r="G30" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="31" spans="3:7">
-      <c r="C31" t="s">
-        <v>115</v>
-      </c>
-      <c r="D31" s="10">
-        <v>21000</v>
-      </c>
-      <c r="G31" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="32" spans="3:7">
-      <c r="C32" t="s">
-        <v>98</v>
-      </c>
-      <c r="G32" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="33" spans="3:7">
-      <c r="C33" t="s">
-        <v>101</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="G33" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="34" spans="3:7">
-      <c r="C34" t="s">
-        <v>116</v>
-      </c>
-      <c r="D34" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="G34" t="s">
-        <v>45</v>
-      </c>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="H33" s="5"/>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H34" s="3"/>
     </row>
     <row r="35" spans="3:7">
       <c r="C35" t="s">
-        <v>118</v>
+        <v>68</v>
       </c>
       <c r="D35" t="s">
-        <v>107</v>
+        <v>69</v>
       </c>
       <c r="G35" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="3:7">
       <c r="C36" t="s">
-        <v>108</v>
+        <v>70</v>
+      </c>
+      <c r="D36" t="s">
+        <v>71</v>
       </c>
       <c r="G36" t="s">
-        <v>119</v>
-      </c>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="3:7">
+      <c r="C37" t="s">
+        <v>85</v>
+      </c>
+      <c r="F37" t="s">
+        <v>86</v>
+      </c>
+      <c r="G37" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="38" spans="3:8">
+      <c r="C38" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="H38" s="8"/>
+    </row>
+    <row r="39" spans="3:8">
+      <c r="C39" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="H39" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="C1:G1"/>
     <mergeCell ref="D2:F2"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="D33:F33"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:J51"/>
+  <sheetViews>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="43.4285714285714" customWidth="1"/>
+    <col min="3" max="3" width="46" customWidth="1"/>
+    <col min="4" max="4" width="16.5714285714286" customWidth="1"/>
+    <col min="5" max="6" width="16.4285714285714" customWidth="1"/>
+    <col min="7" max="7" width="51.8571428571429" customWidth="1"/>
+    <col min="8" max="8" width="17.8571428571429" customWidth="1"/>
+    <col min="9" max="9" width="37.7142857142857" customWidth="1"/>
+    <col min="10" max="10" width="24.4285714285714" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="3:7">
+      <c r="C4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7">
+      <c r="C5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7">
+      <c r="C6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F6" t="s">
+        <v>86</v>
+      </c>
+      <c r="G6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7">
+      <c r="C7" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="E7" t="s">
+        <v>133</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7">
+      <c r="C8" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D8" t="s">
+        <v>136</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7">
+      <c r="C9" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7">
+      <c r="C10" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7">
+      <c r="C11" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="F11" t="s">
+        <v>143</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7">
+      <c r="C12" s="8"/>
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="3:3">
+      <c r="C13" s="8"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" spans="3:7">
+      <c r="C17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" t="s">
+        <v>69</v>
+      </c>
+      <c r="G17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7">
+      <c r="C18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" t="s">
+        <v>71</v>
+      </c>
+      <c r="G18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7">
+      <c r="C19" t="s">
+        <v>130</v>
+      </c>
+      <c r="F19" t="s">
+        <v>86</v>
+      </c>
+      <c r="G19" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7">
+      <c r="C20" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D20" t="s">
+        <v>147</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7">
+      <c r="C21" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="E21" t="s">
+        <v>150</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7">
+      <c r="C22" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="D22" t="s">
+        <v>44</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7">
+      <c r="C23" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D23" t="s">
+        <v>47</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="24" spans="3:10">
+      <c r="C24" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="F24" t="s">
+        <v>143</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="J24" s="8"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J27" s="8"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="8"/>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="8"/>
+    </row>
+    <row r="30" spans="3:10">
+      <c r="C30" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" t="s">
+        <v>69</v>
+      </c>
+      <c r="G30" t="s">
+        <v>35</v>
+      </c>
+      <c r="J30" s="8"/>
+    </row>
+    <row r="31" spans="3:10">
+      <c r="C31" t="s">
+        <v>70</v>
+      </c>
+      <c r="D31" t="s">
+        <v>71</v>
+      </c>
+      <c r="G31" t="s">
+        <v>72</v>
+      </c>
+      <c r="J31" s="8"/>
+    </row>
+    <row r="32" spans="3:10">
+      <c r="C32" t="s">
+        <v>130</v>
+      </c>
+      <c r="F32" t="s">
+        <v>86</v>
+      </c>
+      <c r="G32" t="s">
+        <v>131</v>
+      </c>
+      <c r="J32" s="8"/>
+    </row>
+    <row r="33" spans="3:10">
+      <c r="C33" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D33" t="s">
+        <v>147</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="J33" s="8"/>
+    </row>
+    <row r="34" spans="3:10">
+      <c r="C34" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D34" t="s">
+        <v>136</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="J34" s="8"/>
+    </row>
+    <row r="35" spans="3:7">
+      <c r="C35" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="E35" t="s">
+        <v>154</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="36" spans="3:7">
+      <c r="C36" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D36" t="s">
+        <v>47</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="37" spans="3:7">
+      <c r="C37" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="F37" t="s">
+        <v>143</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="4"/>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+    </row>
+    <row r="43" spans="3:7">
+      <c r="C43" t="s">
+        <v>68</v>
+      </c>
+      <c r="D43" t="s">
+        <v>69</v>
+      </c>
+      <c r="G43" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" customHeight="1" spans="3:7">
+      <c r="C44" t="s">
+        <v>70</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="G44" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="45" spans="3:7">
+      <c r="C45" t="s">
+        <v>130</v>
+      </c>
+      <c r="F45" t="s">
+        <v>86</v>
+      </c>
+      <c r="G45" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="46" spans="3:7">
+      <c r="C46" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D46" t="s">
+        <v>147</v>
+      </c>
+      <c r="G46" s="8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="47" spans="3:7">
+      <c r="C47" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D47" t="s">
+        <v>136</v>
+      </c>
+      <c r="G47" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="48" spans="3:7">
+      <c r="C48" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="D48" t="s">
+        <v>44</v>
+      </c>
+      <c r="G48" s="8" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="49" spans="3:7">
+      <c r="C49" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D49" t="s">
+        <v>47</v>
+      </c>
+      <c r="G49" s="8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="50" customFormat="1" spans="3:7">
+      <c r="C50" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="E50" t="s">
+        <v>160</v>
+      </c>
+      <c r="G50" s="8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="51" spans="3:7">
+      <c r="C51" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="F51" t="s">
+        <v>143</v>
+      </c>
+      <c r="G51" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="C40:G40"/>
+    <mergeCell ref="D41:F41"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D44" r:id="rId1" display="http://automationpractice.com/index.php?controller=my-account"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:J48"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A19" sqref="$A19:$XFD19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="43.4285714285714" customWidth="1"/>
+    <col min="3" max="3" width="46" customWidth="1"/>
+    <col min="4" max="4" width="16.5714285714286" customWidth="1"/>
+    <col min="5" max="6" width="16.4285714285714" customWidth="1"/>
+    <col min="7" max="7" width="51.8571428571429" customWidth="1"/>
+    <col min="8" max="8" width="17.8571428571429" customWidth="1"/>
+    <col min="9" max="9" width="37.7142857142857" customWidth="1"/>
+    <col min="10" max="10" width="24.4285714285714" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="3:7">
+      <c r="C4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7">
+      <c r="C5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="G5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7">
+      <c r="C6" t="s">
+        <v>163</v>
+      </c>
+      <c r="F6" t="s">
+        <v>86</v>
+      </c>
+      <c r="G6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7">
+      <c r="C7" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7">
+      <c r="C8" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7">
+      <c r="C9" s="8"/>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="3:7">
+      <c r="C10" s="8"/>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="3:7">
+      <c r="C14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" t="s">
+        <v>69</v>
+      </c>
+      <c r="G14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="3:7">
+      <c r="C15" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="G15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="3:7">
+      <c r="C16" t="s">
+        <v>163</v>
+      </c>
+      <c r="F16" t="s">
+        <v>86</v>
+      </c>
+      <c r="G16" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7">
+      <c r="C17" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D17" t="s">
+        <v>172</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7">
+      <c r="C18" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7">
+      <c r="C19" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D19" t="s">
+        <v>173</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7">
+      <c r="C20" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7">
+      <c r="C21" s="8"/>
+      <c r="G21" s="8"/>
+    </row>
+    <row r="22" spans="3:7">
+      <c r="C22" s="8"/>
+      <c r="G22" s="8"/>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+    </row>
+    <row r="26" spans="3:7">
+      <c r="C26" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" t="s">
+        <v>69</v>
+      </c>
+      <c r="G26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="3:7">
+      <c r="C27" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="G27" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" customFormat="1" spans="3:7">
+      <c r="C28" t="s">
+        <v>163</v>
+      </c>
+      <c r="F28" t="s">
+        <v>86</v>
+      </c>
+      <c r="G28" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="29" spans="3:7">
+      <c r="C29" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="30" spans="3:7">
+      <c r="C30" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="F30" t="s">
+        <v>180</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="9"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="8"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="8"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="8"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="8"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="8"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="8"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="8"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="8"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="8"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="8"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="8"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" s="8"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" s="8"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8"/>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" s="8"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="8"/>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" s="8"/>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="8"/>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" s="8"/>
+      <c r="B48" s="8"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="D24:F24"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D5" r:id="rId1" display="http://automationpractice.com/index.php?controller=my-account"/>
+    <hyperlink ref="D15" r:id="rId1" display="http://automationpractice.com/index.php?controller=my-account"/>
+    <hyperlink ref="D27" r:id="rId1" display="http://automationpractice.com/index.php?controller=my-account"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>